<commit_message>
idk what github is doing here
</commit_message>
<xml_diff>
--- a/Data/IndividualCounties/RegressionOverview.xlsx
+++ b/Data/IndividualCounties/RegressionOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guslipkin/Documents/COVID-TimeSeries-GIS/Data/IndividualCounties/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14452048-184E-B149-AD8B-6426365AB6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CBDA01-B70A-4946-8B33-2AC7B6E8CAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{5099255D-7498-844E-9A02-E719D1D7C3E3}"/>
   </bookViews>
@@ -994,7 +994,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,297 +1038,297 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2">
-        <v>13277</v>
+        <v>4019</v>
       </c>
       <c r="C2">
-        <v>8.0111892425927853E-2</v>
+        <v>0.26790685895092164</v>
       </c>
       <c r="D2">
-        <v>0.60063760341209671</v>
+        <v>0.33439461718401181</v>
       </c>
       <c r="E2">
-        <v>0.48833484129302895</v>
+        <v>0.97643933590784338</v>
       </c>
       <c r="F2">
-        <v>0.54666331329560613</v>
+        <v>0.26287927175163278</v>
       </c>
       <c r="G2">
-        <v>40571</v>
+        <v>1039073</v>
       </c>
       <c r="H2">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="I2">
-        <v>5046</v>
+        <v>118938</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3">
-        <v>22083</v>
+        <v>6075</v>
       </c>
       <c r="C3">
-        <v>0.11374960798535155</v>
+        <v>0.21277399384550263</v>
       </c>
       <c r="D3">
-        <v>0.36307953415092936</v>
+        <v>0.30105977581628607</v>
       </c>
       <c r="E3">
-        <v>0.55731974446905652</v>
+        <v>0.40027998752398364</v>
       </c>
       <c r="F3">
-        <v>0.45032470711583328</v>
+        <v>0.716326082603706</v>
       </c>
       <c r="G3">
-        <v>20192</v>
+        <v>883305</v>
       </c>
       <c r="H3">
-        <v>36</v>
+        <v>18790.740000000002</v>
       </c>
       <c r="I3">
-        <v>2597</v>
+        <v>38367</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4">
-        <v>6075</v>
+        <v>12086</v>
       </c>
       <c r="C4">
-        <v>0.21277399384550263</v>
+        <v>0.3735087171580328</v>
       </c>
       <c r="D4">
-        <v>0.30105977581628607</v>
+        <v>0.25076116701202689</v>
       </c>
       <c r="E4">
-        <v>0.40027998752398364</v>
+        <v>0.52415012309684905</v>
       </c>
       <c r="F4">
-        <v>0.716326082603706</v>
+        <v>0.2122560295182917</v>
       </c>
       <c r="G4">
-        <v>883305</v>
+        <v>2761581</v>
       </c>
       <c r="H4">
-        <v>18790.740000000002</v>
+        <v>1000</v>
       </c>
       <c r="I4">
-        <v>38367</v>
+        <v>522734</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5">
-        <v>4019</v>
+        <v>13277</v>
       </c>
       <c r="C5">
-        <v>0.26790685895092164</v>
+        <v>8.0111892425927853E-2</v>
       </c>
       <c r="D5">
-        <v>0.33439461718401181</v>
+        <v>0.60063760341209671</v>
       </c>
       <c r="E5">
-        <v>0.97643933590784338</v>
+        <v>0.48833484129302895</v>
       </c>
       <c r="F5">
-        <v>0.26287927175163278</v>
+        <v>0.54666331329560613</v>
       </c>
       <c r="G5">
-        <v>1039073</v>
+        <v>40571</v>
       </c>
       <c r="H5">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="I5">
-        <v>118938</v>
+        <v>5046</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6">
-        <v>45083</v>
+        <v>17031</v>
       </c>
       <c r="C6">
-        <v>0.30933900600000003</v>
+        <v>0.76268883815709054</v>
       </c>
       <c r="D6">
-        <v>0.10048436778107525</v>
+        <v>6.9182217375742625E-3</v>
       </c>
       <c r="E6">
-        <v>0.19534937661599464</v>
+        <v>1.6098642687428766E-3</v>
       </c>
       <c r="F6">
-        <v>0.21356770142554041</v>
+        <v>0.22655310551267324</v>
       </c>
       <c r="G6">
-        <v>313888</v>
+        <v>5180493</v>
       </c>
       <c r="H6">
-        <v>350</v>
+        <v>5450</v>
       </c>
       <c r="I6">
-        <v>42302</v>
+        <v>559767</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B7">
-        <v>12086</v>
+        <v>22083</v>
       </c>
       <c r="C7">
-        <v>0.3735087171580328</v>
+        <v>0.11374960798535155</v>
       </c>
       <c r="D7">
-        <v>0.25076116701202689</v>
+        <v>0.36307953415092936</v>
       </c>
       <c r="E7">
-        <v>0.52415012309684905</v>
+        <v>0.55731974446905652</v>
       </c>
       <c r="F7">
-        <v>0.2122560295182917</v>
+        <v>0.45032470711583328</v>
       </c>
       <c r="G7">
-        <v>2761581</v>
+        <v>20192</v>
       </c>
       <c r="H7">
-        <v>1000</v>
+        <v>36</v>
       </c>
       <c r="I7">
-        <v>522734</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8">
-        <v>48315</v>
+        <v>36061</v>
       </c>
       <c r="C8">
-        <v>0.38347786524491162</v>
+        <v>0.39831268309002121</v>
       </c>
       <c r="D8">
-        <v>0.9360000865471243</v>
+        <v>0.88800432651832428</v>
       </c>
       <c r="E8">
-        <v>0.10936240698983132</v>
+        <v>0.17927838738967278</v>
       </c>
       <c r="F8">
-        <v>8.9534097425320217E-2</v>
+        <v>0.98352732191069203</v>
       </c>
       <c r="G8">
-        <v>9928</v>
+        <v>1628701</v>
       </c>
       <c r="H8">
-        <v>28</v>
+        <v>69467.5</v>
       </c>
       <c r="I8">
-        <v>637</v>
+        <v>140314</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9">
-        <v>36061</v>
+        <v>39103</v>
       </c>
       <c r="C9">
-        <v>0.39831268309002121</v>
+        <v>0.61505672040613568</v>
       </c>
       <c r="D9">
-        <v>0.88800432651832428</v>
+        <v>8.2673880820460545E-3</v>
       </c>
       <c r="E9">
-        <v>0.17927838738967278</v>
+        <v>3.4704768663951668E-2</v>
       </c>
       <c r="F9">
-        <v>0.98352732191069203</v>
+        <v>3.3278946466456856E-2</v>
       </c>
       <c r="G9">
-        <v>1628701</v>
+        <v>179146</v>
       </c>
       <c r="H9">
-        <v>69467.5</v>
+        <v>2240.87</v>
       </c>
       <c r="I9">
-        <v>140314</v>
+        <v>15744</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10">
-        <v>39103</v>
+        <v>45083</v>
       </c>
       <c r="C10">
-        <v>0.61505672040613568</v>
+        <v>0.30933900600000003</v>
       </c>
       <c r="D10">
-        <v>8.2673880820460545E-3</v>
+        <v>0.10048436778107525</v>
       </c>
       <c r="E10">
-        <v>3.4704768663951668E-2</v>
+        <v>0.19534937661599464</v>
       </c>
       <c r="F10">
-        <v>3.3278946466456856E-2</v>
+        <v>0.21356770142554041</v>
       </c>
       <c r="G10">
-        <v>179146</v>
+        <v>313888</v>
       </c>
       <c r="H10">
-        <v>2240.87</v>
+        <v>350</v>
       </c>
       <c r="I10">
-        <v>15744</v>
+        <v>42302</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B11">
-        <v>17031</v>
+        <v>48315</v>
       </c>
       <c r="C11">
-        <v>0.76268883815709054</v>
+        <v>0.38347786524491162</v>
       </c>
       <c r="D11">
-        <v>6.9182217375742625E-3</v>
+        <v>0.9360000865471243</v>
       </c>
       <c r="E11">
-        <v>1.6098642687428766E-3</v>
+        <v>0.10936240698983132</v>
       </c>
       <c r="F11">
-        <v>0.22655310551267324</v>
+        <v>8.9534097425320217E-2</v>
       </c>
       <c r="G11">
-        <v>5180493</v>
+        <v>9928</v>
       </c>
       <c r="H11">
-        <v>5450</v>
+        <v>28</v>
       </c>
       <c r="I11">
-        <v>559767</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I11">
-    <sortCondition ref="C1:C11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
+    <sortCondition ref="B1:B12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>